<commit_message>
Added precalculated Resnik scores and dropped ``phenopy`` dependency.
</commit_message>
<xml_diff>
--- a/phenoscore/sample_data/random_generated_sample_data.xlsx
+++ b/phenoscore/sample_data/random_generated_sample_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Genetica Projecten\Facial Recognition\Studenten en Onderzoekers\Lex\Projecten\FaceReader\Github_upload_both\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Z184215\Documents\H_schijf_Lex\Projecten\FaceReader\Scripts\PhenoScore\PhenoScore\phenoscore\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14734FD8-81F7-424C-9815-2518B71367AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378AAAB2-ABEB-4838-A313-C5791F2F224D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>ind_10.png</t>
   </si>
   <si>
-    <t>['HP:0012520', 'HP:0002266', 'HP:0010651', 'HP:0020219', 'HP:0012379', 'HP:0007301', 'HP:0000098', 'HP:0002926', 'HP:0011195', 'HP:0001707', 'HP:0004323', 'HP:0011122', 'HP:0007598', 'HP:0010787', 'HP:0002286', 'HP:0100818', 'HP:0002121', 'HP:0001010', 'HP:0010719', 'HP:0000505', 'HP:0001533', 'HP:0000470', 'HP:0040195', 'HP:0001508', 'HP:0002373', 'HP:0000078', 'HP:0011360']</t>
-  </si>
-  <si>
     <t>['HP:0010866', 'HP:0003043', 'HP:0031567', 'HP:0000954', 'HP:0009811', 'HP:0020219', 'HP:0001881', 'HP:0000846', 'HP:0030311']</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>['HP:0001511', 'HP:0000277', 'HP:0011410', 'HP:0000951', 'HP:0001027', 'HP:0001342', 'HP:0011138', 'HP:0001388', 'HP:0000818', 'HP:0002904', 'HP:0008689', 'HP:0003319', 'HP:0000577', 'HP:0006698', 'HP:0100806', 'HP:0000960', 'HP:0000001', 'HP:0033019', 'HP:0002213']</t>
   </si>
   <si>
-    <t>['HP:0031938', 'HP:0011282', 'HP:0000347', 'HP:0200043', 'HP:0001551', 'HP:0040195', 'HP:0025015', 'HP:0001762', 'HP:0003265', 'HP:0005164', 'HP:0000268', 'HP:0001933', 'HP:0011329', 'HP:0001647', 'HP:0001671']</t>
-  </si>
-  <si>
     <t>['HP:0001388', 'HP:0002996', 'HP:0002299', 'HP:0000821', 'HP:0002205', 'HP:0001877', 'HP:0000826', 'HP:0000750', 'HP:0001376', 'HP:0001511', 'HP:0001317', 'HP:0033127', 'HP:0002813', 'HP:0002059', 'HP:0001288', 'HP:0002087', 'HP:0012503', 'HP:0002518', 'HP:0001421', 'HP:0007369']</t>
   </si>
   <si>
@@ -154,6 +148,12 @@
   </si>
   <si>
     <t>path_to_file</t>
+  </si>
+  <si>
+    <t>['HP:0012520', 'HP:0000709', 'HP:0002266', 'HP:0010651', 'HP:0020219', 'HP:0012379', 'HP:0007301', 'HP:0000098', 'HP:0002926', 'HP:0011195', 'HP:0001707', 'HP:0004323', 'HP:0011122', 'HP:0007598', 'HP:0010787', 'HP:0002286', 'HP:0100818', 'HP:0002121', 'HP:0001010', 'HP:0010719', 'HP:0000505', 'HP:0001533', 'HP:0000470', 'HP:0040195', 'HP:0001508', 'HP:0002373', 'HP:0000078', 'HP:0011360']</t>
+  </si>
+  <si>
+    <t>['HP:0031938', 'HP:0011282', 'HP:0000582', 'HP:0000347', 'HP:0200043', 'HP:0001551', 'HP:0040195', 'HP:0025015', 'HP:0001762', 'HP:0003265', 'HP:0005164', 'HP:0000268', 'HP:0001933', 'HP:0011329', 'HP:0001647', 'HP:0001671']</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,13 +485,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -543,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -565,7 +565,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -576,7 +576,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -587,7 +587,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -598,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -609,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -620,7 +620,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -631,7 +631,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -642,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -653,7 +653,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -664,7 +664,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -675,7 +675,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -686,7 +686,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -697,7 +697,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -708,7 +708,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>1</v>

</xml_diff>